<commit_message>
Signed-off-by: Kalyan Chakravarthi Mundra <km028941@broadcom.net>
</commit_message>
<xml_diff>
--- a/data/3DS_SanityClearCardTestData.xlsx
+++ b/data/3DS_SanityClearCardTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12290" windowHeight="4100" tabRatio="997" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12290" windowHeight="4100" tabRatio="997" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TEST SCENARIOS" sheetId="1" r:id="rId1"/>
@@ -951,9 +951,6 @@
     <t>AAAAAA123456789</t>
   </si>
   <si>
-    <t>12345678912</t>
-  </si>
-  <si>
     <t>AcquirerMerchantID222</t>
   </si>
   <si>
@@ -1651,9 +1648,6 @@
 }</t>
   </si>
   <si>
-    <t>4000500060000008</t>
-  </si>
-  <si>
     <t>CA_EU</t>
   </si>
   <si>
@@ -1664,9 +1658,6 @@
   </si>
   <si>
     <t>340000000001007</t>
-  </si>
-  <si>
-    <t>5186003100001014</t>
   </si>
   <si>
     <t>_A001</t>
@@ -1690,13 +1681,7 @@
    "callerTxnRefID": "#callerTxnRefID#"}</t>
   </si>
   <si>
-    <t>CADS</t>
-  </si>
-  <si>
     <t>Stephen</t>
-  </si>
-  <si>
-    <t>300</t>
   </si>
   <si>
     <t>{
@@ -1828,9 +1813,6 @@
 }</t>
   </si>
   <si>
-    <t>350</t>
-  </si>
-  <si>
     <t>BRW_AReq_API_ByPass3DSMethodurl</t>
   </si>
   <si>
@@ -2004,6 +1986,24 @@
   </si>
   <si>
     <t>_SanityFrictionless_Sample Valid Areq Request</t>
+  </si>
+  <si>
+    <t>MTD000000</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>5200000000001005</t>
+  </si>
+  <si>
+    <t>4000000000001000</t>
+  </si>
+  <si>
+    <t>DsReferenceNumber</t>
+  </si>
+  <si>
+    <t>35000</t>
   </si>
 </sst>
 </file>
@@ -2582,7 +2582,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>6</v>
@@ -2593,43 +2593,43 @@
         <v>154</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="289.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="289.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="289.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="391.5" x14ac:dyDescent="0.35">
@@ -2637,10 +2637,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
@@ -2651,40 +2651,40 @@
         <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="289.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2696,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2732,31 +2732,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>81</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -2777,31 +2777,31 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2813,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CD2" sqref="CD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2979,91 +2979,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -3366,51 +3366,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -3421,73 +3421,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -3496,10 +3496,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -3553,7 +3553,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -3613,7 +3613,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -3646,7 +3646,7 @@
         <v>33</v>
       </c>
       <c r="CD2" s="11" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="CE2" s="11" t="s">
         <v>15</v>
@@ -3658,10 +3658,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -3710,22 +3710,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -3734,31 +3734,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -3794,7 +3794,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -3803,7 +3803,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -3834,8 +3834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CD2" sqref="CD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4000,91 +4000,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -4387,51 +4387,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -4442,73 +4442,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -4517,10 +4517,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -4574,7 +4574,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -4634,7 +4634,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -4667,7 +4667,7 @@
         <v>33</v>
       </c>
       <c r="CD2" s="11" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="CE2" s="11" t="s">
         <v>15</v>
@@ -4679,10 +4679,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -4731,22 +4731,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -4755,31 +4755,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -4815,7 +4815,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -4824,7 +4824,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -4855,8 +4855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CD2" sqref="CD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5021,91 +5021,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -5408,51 +5408,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -5463,73 +5463,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -5538,10 +5538,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -5595,7 +5595,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -5655,7 +5655,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -5688,7 +5688,7 @@
         <v>33</v>
       </c>
       <c r="CD2" s="11" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="CE2" s="11" t="s">
         <v>15</v>
@@ -5700,10 +5700,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -5752,22 +5752,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -5776,31 +5776,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -5836,7 +5836,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -5845,7 +5845,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -5935,61 +5935,61 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>176</v>
-      </c>
       <c r="J1" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>236</v>
-      </c>
       <c r="N1" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="P1" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="Q1" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="S1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="T1" s="31" t="s">
         <v>195</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>196</v>
       </c>
       <c r="U1" s="17" t="s">
         <v>120</v>
       </c>
       <c r="V1" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="W1" s="17" t="s">
         <v>197</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>198</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>80</v>
@@ -6004,22 +6004,22 @@
         <v>99</v>
       </c>
       <c r="AB1" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC1" s="14" t="s">
         <v>199</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>200</v>
       </c>
       <c r="AD1" s="14" t="s">
         <v>135</v>
       </c>
       <c r="AE1" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="AF1" s="29" t="s">
+      <c r="AG1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="AG1" s="29" t="s">
-        <v>224</v>
       </c>
       <c r="AH1" s="14" t="s">
         <v>136</v>
@@ -6028,15 +6028,15 @@
         <v>137</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -6047,46 +6047,46 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="W2" s="11" t="s">
         <v>8</v>
@@ -6095,7 +6095,7 @@
         <v>8</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z2" s="11"/>
       <c r="AA2" s="11"/>
@@ -6103,7 +6103,7 @@
         <v>0</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>21</v>
@@ -6118,13 +6118,13 @@
         <v>18</v>
       </c>
       <c r="AH2" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AJ2" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -6187,84 +6187,84 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="W1" s="17" t="s">
         <v>99</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z1" s="17" t="s">
         <v>81</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AB1" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -6275,63 +6275,63 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W2" s="11"/>
       <c r="X2" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y2" s="36"/>
       <c r="Z2" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>0</v>
@@ -6401,22 +6401,22 @@
         <v>1</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I7" s="41"/>
       <c r="J7" s="42"/>
       <c r="L7" s="40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M7" s="41"/>
       <c r="N7" s="42"/>
       <c r="P7" s="40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q7" s="41"/>
       <c r="R7" s="42"/>
       <c r="T7" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U7" s="41"/>
       <c r="V7" s="42"/>
@@ -6427,31 +6427,31 @@
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="N8" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="N8" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="P8" s="21"/>
       <c r="Q8" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="R8" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="T8" s="21"/>
       <c r="U8" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="V8" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="V8" s="22" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -6459,7 +6459,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I9" s="21">
         <v>550</v>
@@ -6468,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M9" s="35">
         <v>517</v>
@@ -6477,7 +6477,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q9" s="35">
         <v>390</v>
@@ -6486,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U9" s="21">
         <v>87</v>
@@ -6500,7 +6500,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I10" s="21">
         <v>458</v>
@@ -6509,7 +6509,7 @@
         <v>92</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M10" s="21">
         <v>376</v>
@@ -6518,7 +6518,7 @@
         <v>141</v>
       </c>
       <c r="P10" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q10" s="21">
         <v>266</v>
@@ -6527,7 +6527,7 @@
         <v>124</v>
       </c>
       <c r="T10" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U10" s="21">
         <v>87</v>
@@ -6541,7 +6541,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I9:I10)</f>
@@ -6552,7 +6552,7 @@
         <v>92</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M11" s="23">
         <f>SUM(M9:M10)</f>
@@ -6563,7 +6563,7 @@
         <v>141</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q11" s="23">
         <f>SUM(Q9:Q10)</f>
@@ -6574,7 +6574,7 @@
         <v>124</v>
       </c>
       <c r="T11" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U11" s="23">
         <f>SUM(U9:U10)</f>
@@ -6590,7 +6590,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I12" s="27">
         <f>I11/(I11+J11)</f>
@@ -6601,7 +6601,7 @@
         <v>8.3636363636363634E-2</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M12" s="27">
         <f>M11/(M11+N11)</f>
@@ -6612,7 +6612,7 @@
         <v>0.13636363636363635</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q12" s="27">
         <f>Q11/(Q11+R11)</f>
@@ -6623,7 +6623,7 @@
         <v>0.15897435897435896</v>
       </c>
       <c r="T12" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U12" s="27">
         <f>U11/(U11+V11)</f>
@@ -6650,7 +6650,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M15" s="38"/>
       <c r="N15" s="39"/>
@@ -6661,10 +6661,10 @@
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="N16" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="N16" s="22" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M17" s="21">
         <f>SUM(I9+M9+Q9+U9)</f>
@@ -6688,7 +6688,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M18" s="21">
         <f>SUM(I10+M10+Q10+U10)</f>
@@ -6704,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M19" s="23">
         <f>SUM(M17:M18)</f>
@@ -6720,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M20" s="27">
         <f>M19/(M19+N19)</f>
@@ -9282,7 +9282,7 @@
       </c>
       <c r="L530" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>77ee4605-76bd-9466-42fa-412e91124bc4</v>
+        <v>214f37d5-a19a-67df-3a6f-ce2d3259699b</v>
       </c>
     </row>
     <row r="531" spans="1:12" x14ac:dyDescent="0.35">
@@ -9291,7 +9291,7 @@
       </c>
       <c r="L531" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>01d09994-7a1b-6617-a280-f4050e4977d7</v>
+        <v>aa85c436-1334-9aa3-3565-f8da64b367a8</v>
       </c>
     </row>
     <row r="532" spans="1:12" x14ac:dyDescent="0.35">
@@ -9300,7 +9300,7 @@
       </c>
       <c r="L532" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>2b363252-a3c6-019e-7b68-d28bf2308ba9</v>
+        <v>143f9b33-2e24-a6d4-237d-07dde81623ba</v>
       </c>
     </row>
     <row r="533" spans="1:12" x14ac:dyDescent="0.35">
@@ -9452,31 +9452,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>81</v>
@@ -9484,10 +9484,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -9497,31 +9497,31 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -9535,8 +9535,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9571,31 +9571,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>81</v>
@@ -9603,10 +9603,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -9616,31 +9616,31 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -9654,8 +9654,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9690,31 +9690,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>81</v>
@@ -9722,10 +9722,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -9735,31 +9735,31 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -9773,9 +9773,9 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9940,91 +9940,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -10327,51 +10327,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -10382,73 +10382,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -10457,10 +10457,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -10514,7 +10514,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -10574,7 +10574,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -10619,10 +10619,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -10671,22 +10671,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -10695,31 +10695,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -10755,7 +10755,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -10764,7 +10764,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -10797,9 +10797,9 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10964,91 +10964,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -11351,51 +11351,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -11406,73 +11406,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -11481,10 +11481,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -11538,7 +11538,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -11598,7 +11598,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -11643,10 +11643,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -11695,22 +11695,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -11719,31 +11719,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -11779,7 +11779,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -11788,7 +11788,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -11821,9 +11821,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11988,91 +11988,91 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>173</v>
-      </c>
       <c r="AD1" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH1" s="17" t="s">
         <v>40</v>
@@ -12375,51 +12375,51 @@
         <v>139</v>
       </c>
       <c r="ED1" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="EE1" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EF1" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="EF1" s="14" t="s">
+      <c r="EG1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="EG1" s="29" t="s">
+      <c r="EH1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="EH1" s="29" t="s">
+      <c r="EI1" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="EI1" s="29" t="s">
+      <c r="EJ1" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="EJ1" s="29" t="s">
+      <c r="EK1" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="EK1" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="EL1" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="EM1" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="EM1" s="29" t="s">
+      <c r="EN1" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="EN1" s="29" t="s">
+      <c r="EO1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="EO1" s="29" t="s">
+      <c r="EP1" s="29" t="s">
         <v>223</v>
-      </c>
-      <c r="EP1" s="29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -12430,73 +12430,73 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="U2" s="11" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Y2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>22</v>
@@ -12505,10 +12505,10 @@
         <v>11</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>7</v>
@@ -12562,7 +12562,7 @@
         <v>35</v>
       </c>
       <c r="AY2" s="11" t="s">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="AZ2" s="11" t="s">
         <v>8</v>
@@ -12622,7 +12622,7 @@
         <v>28</v>
       </c>
       <c r="BS2" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="BT2" s="11" t="s">
         <v>9</v>
@@ -12667,10 +12667,10 @@
         <v>30</v>
       </c>
       <c r="CH2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CI2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CJ2" s="11" t="s">
         <v>143</v>
@@ -12719,22 +12719,22 @@
         <v>8</v>
       </c>
       <c r="CZ2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DA2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="DB2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="DC2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="DD2" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="DE2" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="DE2" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="DF2" s="16" t="s">
         <v>155</v>
@@ -12743,31 +12743,31 @@
         <v>158</v>
       </c>
       <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="DJ2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="DK2" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="DK2" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="DL2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="DM2" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DN2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="DO2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="DP2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="DQ2" s="16" t="s">
         <v>134</v>
@@ -12803,7 +12803,7 @@
         <v>138</v>
       </c>
       <c r="EB2" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="EC2" s="11" t="s">
         <v>8</v>
@@ -12812,7 +12812,7 @@
       <c r="EE2" s="11"/>
       <c r="EF2" s="11"/>
       <c r="EG2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EH2" s="11"/>
       <c r="EI2" s="11"/>
@@ -12841,123 +12841,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -12997,31 +12880,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>245</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>81</v>
@@ -13029,10 +12912,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>0</v>
@@ -13042,31 +12925,148 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>271</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>269</v>
+      </c>
       <c r="M2" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commting the TestData for
Example :
"homePhone": {
  "cc": "1",
  "subscriber": "1234567973"
},
"workPhone": {
  "cc": "1",
  "subscriber": "1234567973"
},
"mobilePhone": {
  "cc": "1",
  "subscriber": "1234567973"
}
</commit_message>
<xml_diff>
--- a/data/3DS_SanityClearCardTestData.xlsx
+++ b/data/3DS_SanityClearCardTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12290" windowHeight="4100" tabRatio="997" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12290" windowHeight="4100" tabRatio="997" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TEST SCENARIOS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'4_VERIFY'!$A$1:$AA$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'4_VMURL_V'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2813,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD2" sqref="CD2"/>
+    <sheetView topLeftCell="BU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BZ11" sqref="BZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3622,7 +3622,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -3637,7 +3637,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>
@@ -3834,8 +3834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD2" sqref="CD2"/>
+    <sheetView topLeftCell="BU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BY10" sqref="BY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4643,7 +4643,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -4658,7 +4658,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>
@@ -4855,8 +4855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD2" sqref="CD2"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BY10" sqref="BY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5664,7 +5664,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -5679,7 +5679,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -5731,7 +5731,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>
@@ -9282,7 +9282,7 @@
       </c>
       <c r="L530" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>214f37d5-a19a-67df-3a6f-ce2d3259699b</v>
+        <v>4ecb24fc-72b7-89fb-6572-b3e7379f72ea</v>
       </c>
     </row>
     <row r="531" spans="1:12" x14ac:dyDescent="0.35">
@@ -9291,7 +9291,7 @@
       </c>
       <c r="L531" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>aa85c436-1334-9aa3-3565-f8da64b367a8</v>
+        <v>1f4d1d5e-8ad1-51c1-0dbb-6942d6d8405e</v>
       </c>
     </row>
     <row r="532" spans="1:12" x14ac:dyDescent="0.35">
@@ -9300,7 +9300,7 @@
       </c>
       <c r="L532" s="33" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>143f9b33-2e24-a6d4-237d-07dde81623ba</v>
+        <v>fdfbc54b-5070-1cd5-52c1-f126dc153cbc</v>
       </c>
     </row>
     <row r="533" spans="1:12" x14ac:dyDescent="0.35">
@@ -9773,9 +9773,9 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="BR1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="BV15" sqref="BV15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10583,7 +10583,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -10598,7 +10598,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -10650,7 +10650,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>
@@ -10797,9 +10797,9 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="BT1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="CA16" sqref="CA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11607,7 +11607,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -11622,7 +11622,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -11674,7 +11674,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>
@@ -11821,9 +11821,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
+    <sheetView topLeftCell="BR1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="BW15" sqref="BW15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12631,7 +12631,7 @@
         <v>134</v>
       </c>
       <c r="BV2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="BW2" s="11" t="s">
         <v>145</v>
@@ -12646,7 +12646,7 @@
         <v>32</v>
       </c>
       <c r="CA2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CB2" s="11" t="s">
         <v>145</v>
@@ -12698,7 +12698,7 @@
       </c>
       <c r="CR2" s="11"/>
       <c r="CS2" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="CT2" s="11" t="s">
         <v>145</v>

</xml_diff>